<commit_message>
modulo 8, avancar com PIP
</commit_message>
<xml_diff>
--- a/observacao.xlsx
+++ b/observacao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24933" windowHeight="11203"/>
+    <workbookView windowWidth="3020" windowHeight="10902"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>Registo de Observação para Avaliação Contínua</t>
   </si>
@@ -58,10 +58,7 @@
     <t>Formando 8</t>
   </si>
   <si>
-    <t>Atenção</t>
-  </si>
-  <si>
-    <t>Participação</t>
+    <t>Participaçao</t>
   </si>
   <si>
     <t>Assiduidade</t>
@@ -93,9 +90,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -141,8 +138,121 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,43 +266,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -200,82 +273,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -292,79 +289,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,96 +464,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,6 +872,80 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,221 +958,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -1556,10 +1553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.45"/>
@@ -1723,66 +1720,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" ht="20" customHeight="1" spans="1:10">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="36"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" ht="20" customHeight="1" spans="1:10">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="37"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" ht="20" customHeight="1" spans="1:10">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="35"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:10">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="38"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" ht="20" customHeight="1" spans="1:10">
       <c r="A15" s="8"/>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1822,24 +1817,23 @@
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" ht="20" customHeight="1" spans="1:10">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="2"/>
+    <row r="19" ht="20" customHeight="1" spans="1:9">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" ht="20" customHeight="1" spans="1:9">
       <c r="A20" s="23"/>
@@ -1847,46 +1841,48 @@
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" ht="20" customHeight="1" spans="1:9">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="23"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" ht="14.2" spans="2:2">
-      <c r="B25" s="2"/>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" ht="50" customHeight="1" spans="1:9">
+      <c r="A25" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" ht="50" customHeight="1" spans="1:9">
-      <c r="A26" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="39"/>
+      <c r="A26" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="40"/>
     </row>
     <row r="27" ht="50" customHeight="1" spans="1:9">
       <c r="A27" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
@@ -1899,7 +1895,7 @@
     </row>
     <row r="28" ht="50" customHeight="1" spans="1:9">
       <c r="A28" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="27"/>
@@ -1912,7 +1908,7 @@
     </row>
     <row r="29" ht="50" customHeight="1" spans="1:9">
       <c r="A29" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
@@ -1925,7 +1921,7 @@
     </row>
     <row r="30" ht="50" customHeight="1" spans="1:9">
       <c r="A30" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="27"/>
@@ -1937,47 +1933,34 @@
       <c r="I30" s="40"/>
     </row>
     <row r="31" ht="50" customHeight="1" spans="1:9">
-      <c r="A31" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="40"/>
+      <c r="A31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" ht="50" customHeight="1" spans="1:9">
-      <c r="A32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="41"/>
-    </row>
-    <row r="33" ht="50" customHeight="1" spans="1:9">
-      <c r="A33" s="30" t="s">
+      <c r="A32" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="42"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="42"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.751388888888889" right="0.751388888888889" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>